<commit_message>
removed mega menu dependency
</commit_message>
<xml_diff>
--- a/src/Data/TestData.xlsx
+++ b/src/Data/TestData.xlsx
@@ -1351,6 +1351,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1362,21 +1377,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3041,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3195,8 +3195,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
+      <c r="A15" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>3</v>
@@ -3224,8 +3224,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
+      <c r="A16" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>3</v>
@@ -3253,8 +3253,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
+      <c r="A17" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>3</v>
@@ -3282,8 +3282,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
+      <c r="A18" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>3</v>
@@ -3358,8 +3358,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
+      <c r="A23" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>3</v>
@@ -3454,7 +3454,7 @@
     <mergeCell ref="A21:C21"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A19 A10 A27:A28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10 A27:A28 A15:A19 A23">
       <formula1>$A$201:$A$202</formula1>
     </dataValidation>
   </dataValidations>
@@ -3534,13 +3534,13 @@
         <v>13</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="61" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3560,9 +3560,9 @@
       <c r="E4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -3624,13 +3624,13 @@
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H8" s="61" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3650,9 +3650,9 @@
       <c r="E9" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="55"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
@@ -3714,13 +3714,13 @@
         <v>15</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="56" t="s">
+      <c r="G13" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="56" t="s">
+      <c r="H13" s="61" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3740,9 +3740,9 @@
       <c r="E14" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
@@ -3804,13 +3804,13 @@
         <v>19</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="56" t="s">
+      <c r="G18" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="56" t="s">
+      <c r="H18" s="61" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3830,9 +3830,9 @@
       <c r="E19" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="55"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
@@ -4106,13 +4106,13 @@
         <v>61</v>
       </c>
       <c r="E35" s="20"/>
-      <c r="F35" s="58" t="s">
+      <c r="F35" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="G35" s="58" t="s">
+      <c r="G35" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="60" t="s">
+      <c r="H35" s="54" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4132,9 +4132,9 @@
       <c r="E36" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="61"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="55"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="22"/>
@@ -4193,13 +4193,13 @@
       <c r="D40" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="60" t="s">
+      <c r="F40" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="G40" s="60" t="s">
+      <c r="G40" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="H40" s="62" t="s">
+      <c r="H40" s="58" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4219,8 +4219,8 @@
       <c r="E41" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
       <c r="H41" s="53"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -4274,13 +4274,13 @@
       <c r="D45" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="60" t="s">
+      <c r="F45" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="G45" s="60" t="s">
+      <c r="G45" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="H45" s="60" t="s">
+      <c r="H45" s="54" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4300,9 +4300,9 @@
       <c r="E46" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
@@ -4355,13 +4355,13 @@
       <c r="D50" t="s">
         <v>83</v>
       </c>
-      <c r="F50" s="60" t="s">
+      <c r="F50" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="60" t="s">
+      <c r="G50" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="H50" s="60" t="s">
+      <c r="H50" s="54" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4381,9 +4381,9 @@
       <c r="E51" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="61"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="23" t="s">
@@ -4436,13 +4436,13 @@
       <c r="D55" t="s">
         <v>92</v>
       </c>
-      <c r="F55" s="60" t="s">
+      <c r="F55" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="G55" s="60" t="s">
+      <c r="G55" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="H55" s="60" t="s">
+      <c r="H55" s="54" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4462,9 +4462,9 @@
       <c r="E56" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="61"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="55"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
@@ -4478,6 +4478,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="H40:H41"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="G55:G56"/>
     <mergeCell ref="H55:H56"/>
@@ -4487,24 +4505,6 @@
     <mergeCell ref="F50:F51"/>
     <mergeCell ref="G50:G51"/>
     <mergeCell ref="H50:H51"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A31 A40:A41 A45:A46 A3:A4 A27 A8:A9 A50:A51 A35:A36 A23 A13:A14 A18:A19 A55:A56">
@@ -6736,10 +6736,10 @@
       <c r="G15" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="I15" s="60" t="s">
+      <c r="I15" s="54" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>